<commit_message>
Update Excel and Work
</commit_message>
<xml_diff>
--- a/Documentos/Tiempo Extra.xlsx
+++ b/Documentos/Tiempo Extra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KCHAVIRA\Documents\GitHub\Wsp-Frames\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90AAE03-DE1D-4F7D-90A7-9E40005C4230}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F60A76C-D0AD-48DC-A38E-B24B6FDB6CBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{B139081F-0435-4DA9-802E-C042E3EDBE3C}"/>
   </bookViews>
@@ -171,7 +171,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0&quot;%&quot;"/>
+    <numFmt numFmtId="164" formatCode="0&quot;%&quot;"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -292,7 +292,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -722,6 +722,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -729,20 +778,11 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -761,18 +801,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -989,21 +1017,6 @@
     <xf numFmtId="44" fontId="2" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1034,12 +1047,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1118,14 +1125,74 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="11" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="11" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1135,25 +1202,6 @@
     <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1179,13 +1227,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -1198,6 +1239,32 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1459,7 +1526,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4148,10 +4214,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{228944A8-6238-4C37-89E8-B94384A08C27}" name="Tabla1" displayName="Tabla1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{228944A8-6238-4C37-89E8-B94384A08C27}" name="Tabla1" displayName="Tabla1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A1:D9" xr:uid="{879F4AD0-DA2A-4013-9B30-AE840B7219E5}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{29C96FE9-AADE-4CD1-8514-4E37564D6A64}" name="Mes" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{29C96FE9-AADE-4CD1-8514-4E37564D6A64}" name="Mes" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{39347D22-2CA3-49C1-BF78-77DEB12A773A}" name="Salarios"/>
     <tableColumn id="3" xr3:uid="{5844BABE-FC05-494E-A614-70E12E0F5DDB}" name="Salarios TE"/>
     <tableColumn id="4" xr3:uid="{6236ABAA-557C-4521-9C74-F24C0B598B59}" name="Total Salarios"/>
@@ -4459,8 +4525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7AE7C4-CD13-4C1B-8581-522CE6888898}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30:L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -4478,651 +4544,713 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="J1" s="119"/>
     </row>
     <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18">
+      <c r="C2" s="10"/>
+      <c r="D2" s="11">
         <v>7</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="11">
         <f>D2*4</f>
         <v>28</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="12">
         <v>220</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="12">
         <f>F2/8</f>
         <v>27.5</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="12">
         <f>2*G2</f>
         <v>55</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2" s="13">
         <f>H2*E2</f>
         <v>1540</v>
       </c>
+      <c r="J2" s="120"/>
     </row>
     <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24">
+      <c r="C3" s="16"/>
+      <c r="D3" s="17">
         <v>8</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="17">
         <f t="shared" ref="E3:E5" si="0">D3*4</f>
         <v>32</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="18">
         <v>225</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="18">
         <f t="shared" ref="G3:G5" si="1">F3/8</f>
         <v>28.125</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="18">
         <f>2*G3</f>
         <v>56.25</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I3" s="19">
         <f>H3*E3</f>
         <v>1800</v>
       </c>
+      <c r="J3" s="120"/>
     </row>
     <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24">
+      <c r="C4" s="16"/>
+      <c r="D4" s="17">
         <v>5</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="17">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="18">
         <v>850</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="18">
         <f t="shared" si="1"/>
         <v>106.25</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="18">
         <f>2*G4</f>
         <v>212.5</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I4" s="19">
         <f>H4*E4</f>
         <v>4250</v>
       </c>
+      <c r="J4" s="120"/>
     </row>
     <row r="5" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="30">
+      <c r="C5" s="22"/>
+      <c r="D5" s="23">
         <v>3</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="23">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="24">
         <v>1200</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="24">
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="24">
         <f>2*G5</f>
         <v>300</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="25">
         <f>H5*E5</f>
         <v>3600</v>
       </c>
+      <c r="J5" s="120"/>
     </row>
     <row r="6" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="8" t="s">
+      <c r="A6" s="122"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="6">
         <f>SUM(I2:I5)</f>
         <v>11190</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="A7" s="122"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="123"/>
+      <c r="H7" s="123"/>
+      <c r="I7" s="123"/>
+      <c r="J7" s="120"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="36">
+      <c r="C8" s="28"/>
+      <c r="D8" s="29">
         <v>9</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="29">
         <f>D8*4</f>
         <v>36</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="30">
         <v>250</v>
       </c>
-      <c r="G8" s="37">
+      <c r="G8" s="30">
         <f>F8/8</f>
         <v>31.25</v>
       </c>
-      <c r="H8" s="37">
+      <c r="H8" s="30">
         <f>2*G8</f>
         <v>62.5</v>
       </c>
-      <c r="I8" s="38">
+      <c r="I8" s="31">
         <f>H8*E8</f>
         <v>2250</v>
       </c>
+      <c r="J8" s="120"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42">
+      <c r="C9" s="34"/>
+      <c r="D9" s="35">
         <v>3</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="35">
         <f t="shared" ref="E9:E10" si="2">D9*4</f>
         <v>12</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="36">
         <v>225</v>
       </c>
-      <c r="G9" s="43">
+      <c r="G9" s="36">
         <f t="shared" ref="G9:G10" si="3">F9/8</f>
         <v>28.125</v>
       </c>
-      <c r="H9" s="43">
+      <c r="H9" s="36">
         <f>2*G9</f>
         <v>56.25</v>
       </c>
-      <c r="I9" s="44">
+      <c r="I9" s="37">
         <f>H9*E9</f>
         <v>675</v>
       </c>
+      <c r="J9" s="120"/>
     </row>
     <row r="10" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="48">
+      <c r="C10" s="40"/>
+      <c r="D10" s="41">
         <v>15</v>
       </c>
-      <c r="E10" s="48">
+      <c r="E10" s="41">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="F10" s="49">
+      <c r="F10" s="42">
         <v>850</v>
       </c>
-      <c r="G10" s="49">
+      <c r="G10" s="42">
         <f t="shared" si="3"/>
         <v>106.25</v>
       </c>
-      <c r="H10" s="49">
+      <c r="H10" s="42">
         <f>2*G10</f>
         <v>212.5</v>
       </c>
-      <c r="I10" s="50">
+      <c r="I10" s="43">
         <f>H10*E10</f>
         <v>12750</v>
       </c>
+      <c r="J10" s="120"/>
     </row>
     <row r="11" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="8" t="s">
+      <c r="A11" s="122"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="123"/>
+      <c r="H11" s="124"/>
+      <c r="I11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="6">
         <f>SUM(I8:I10)</f>
         <v>15675</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="A12" s="125"/>
+      <c r="B12" s="126"/>
+      <c r="C12" s="126"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="124"/>
+      <c r="G12" s="124"/>
+      <c r="H12" s="124"/>
+      <c r="I12" s="126"/>
+      <c r="J12" s="120"/>
     </row>
     <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="54">
+      <c r="C13" s="46"/>
+      <c r="D13" s="47">
         <v>5</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="47">
         <f>D13*4</f>
         <v>20</v>
       </c>
-      <c r="F13" s="55">
+      <c r="F13" s="48">
         <v>220</v>
       </c>
-      <c r="G13" s="55">
+      <c r="G13" s="48">
         <f>F13/8</f>
         <v>27.5</v>
       </c>
-      <c r="H13" s="55">
+      <c r="H13" s="48">
         <f>2*G13</f>
         <v>55</v>
       </c>
-      <c r="I13" s="56">
+      <c r="I13" s="49">
         <f>H13*E13</f>
         <v>1100</v>
       </c>
+      <c r="J13" s="120"/>
     </row>
     <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="59"/>
-      <c r="D14" s="60">
+      <c r="C14" s="52"/>
+      <c r="D14" s="53">
         <v>5</v>
       </c>
-      <c r="E14" s="60">
+      <c r="E14" s="53">
         <f t="shared" ref="E14:E17" si="4">D14*4</f>
         <v>20</v>
       </c>
-      <c r="F14" s="61">
+      <c r="F14" s="54">
         <v>250</v>
       </c>
-      <c r="G14" s="61">
+      <c r="G14" s="54">
         <f t="shared" ref="G14:G17" si="5">F14/8</f>
         <v>31.25</v>
       </c>
-      <c r="H14" s="61">
+      <c r="H14" s="54">
         <f>2*G14</f>
         <v>62.5</v>
       </c>
-      <c r="I14" s="62">
+      <c r="I14" s="55">
         <f>H14*E14</f>
         <v>1250</v>
       </c>
+      <c r="J14" s="120"/>
     </row>
     <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="60">
+      <c r="C15" s="52"/>
+      <c r="D15" s="53">
         <v>5</v>
       </c>
-      <c r="E15" s="60">
+      <c r="E15" s="53">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="F15" s="61">
+      <c r="F15" s="54">
         <v>300</v>
       </c>
-      <c r="G15" s="61">
+      <c r="G15" s="54">
         <f t="shared" si="5"/>
         <v>37.5</v>
       </c>
-      <c r="H15" s="61">
+      <c r="H15" s="54">
         <f>2*G15</f>
         <v>75</v>
       </c>
-      <c r="I15" s="62">
+      <c r="I15" s="55">
         <f>H15*E15</f>
         <v>1500</v>
       </c>
+      <c r="J15" s="120"/>
     </row>
     <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="60">
+      <c r="C16" s="52"/>
+      <c r="D16" s="53">
         <v>3</v>
       </c>
-      <c r="E16" s="60">
+      <c r="E16" s="53">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="F16" s="61">
+      <c r="F16" s="54">
         <v>750</v>
       </c>
-      <c r="G16" s="61">
+      <c r="G16" s="54">
         <f t="shared" si="5"/>
         <v>93.75</v>
       </c>
-      <c r="H16" s="61">
+      <c r="H16" s="54">
         <f>2*G16</f>
         <v>187.5</v>
       </c>
-      <c r="I16" s="62">
+      <c r="I16" s="55">
         <f>H16*E16</f>
         <v>2250</v>
       </c>
+      <c r="J16" s="120"/>
     </row>
     <row r="17" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="65"/>
-      <c r="D17" s="66">
+      <c r="C17" s="58"/>
+      <c r="D17" s="59">
         <v>5</v>
       </c>
-      <c r="E17" s="66">
+      <c r="E17" s="59">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="F17" s="67">
+      <c r="F17" s="60">
         <v>1600</v>
       </c>
-      <c r="G17" s="67">
+      <c r="G17" s="60">
         <f t="shared" si="5"/>
         <v>200</v>
       </c>
-      <c r="H17" s="67">
+      <c r="H17" s="60">
         <f>2*G17</f>
         <v>400</v>
       </c>
-      <c r="I17" s="68">
+      <c r="I17" s="61">
         <f>H17*E17</f>
         <v>8000</v>
       </c>
+      <c r="J17" s="120"/>
     </row>
     <row r="18" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="8" t="s">
+      <c r="A18" s="122"/>
+      <c r="B18" s="80"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="123"/>
+      <c r="G18" s="123"/>
+      <c r="H18" s="124"/>
+      <c r="I18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="6">
         <f>SUM(I13:I17)</f>
         <v>14100</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="A19" s="125"/>
+      <c r="B19" s="126"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="126"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="124"/>
+      <c r="H19" s="124"/>
+      <c r="I19" s="126"/>
+      <c r="J19" s="120"/>
     </row>
     <row r="20" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="70" t="s">
+      <c r="B20" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="71"/>
-      <c r="D20" s="72">
+      <c r="C20" s="64"/>
+      <c r="D20" s="65">
         <v>10</v>
       </c>
-      <c r="E20" s="72">
+      <c r="E20" s="65">
         <f>D20*4</f>
         <v>40</v>
       </c>
-      <c r="F20" s="73">
+      <c r="F20" s="66">
         <v>220</v>
       </c>
-      <c r="G20" s="73">
+      <c r="G20" s="66">
         <f>F20/8</f>
         <v>27.5</v>
       </c>
-      <c r="H20" s="73">
+      <c r="H20" s="66">
         <f>2*G20</f>
         <v>55</v>
       </c>
-      <c r="I20" s="74">
+      <c r="I20" s="67">
         <f>H20*E20</f>
         <v>2200</v>
       </c>
+      <c r="J20" s="120"/>
     </row>
     <row r="21" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="76" t="s">
+      <c r="B21" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="77"/>
-      <c r="D21" s="78">
+      <c r="C21" s="70"/>
+      <c r="D21" s="71">
         <v>10</v>
       </c>
-      <c r="E21" s="78">
+      <c r="E21" s="71">
         <f t="shared" ref="E21:E23" si="6">D21*4</f>
         <v>40</v>
       </c>
-      <c r="F21" s="79">
+      <c r="F21" s="72">
         <v>300</v>
       </c>
-      <c r="G21" s="79">
+      <c r="G21" s="72">
         <f t="shared" ref="G21:G23" si="7">F21/8</f>
         <v>37.5</v>
       </c>
-      <c r="H21" s="79">
+      <c r="H21" s="72">
         <f>2*G21</f>
         <v>75</v>
       </c>
-      <c r="I21" s="80">
+      <c r="I21" s="73">
         <f>H21*E21</f>
         <v>3000</v>
       </c>
+      <c r="J21" s="120"/>
     </row>
     <row r="22" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="75" t="s">
+      <c r="A22" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="76" t="s">
+      <c r="B22" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="77"/>
-      <c r="D22" s="78">
+      <c r="C22" s="70"/>
+      <c r="D22" s="71">
         <v>10</v>
       </c>
-      <c r="E22" s="78">
+      <c r="E22" s="71">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="F22" s="79">
+      <c r="F22" s="72">
         <v>400</v>
       </c>
-      <c r="G22" s="79">
+      <c r="G22" s="72">
         <f t="shared" si="7"/>
         <v>50</v>
       </c>
-      <c r="H22" s="79">
+      <c r="H22" s="72">
         <f>2*G22</f>
         <v>100</v>
       </c>
-      <c r="I22" s="80">
+      <c r="I22" s="73">
         <f>H22*E22</f>
         <v>4000</v>
       </c>
+      <c r="J22" s="120"/>
     </row>
     <row r="23" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="81" t="s">
+      <c r="A23" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="82" t="s">
+      <c r="B23" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="83"/>
-      <c r="D23" s="84">
+      <c r="C23" s="76"/>
+      <c r="D23" s="77">
         <v>0</v>
       </c>
-      <c r="E23" s="84">
+      <c r="E23" s="77">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F23" s="85">
+      <c r="F23" s="78">
         <v>850</v>
       </c>
-      <c r="G23" s="85">
+      <c r="G23" s="78">
         <f t="shared" si="7"/>
         <v>106.25</v>
       </c>
-      <c r="H23" s="85">
+      <c r="H23" s="78">
         <f>2*G23</f>
         <v>212.5</v>
       </c>
-      <c r="I23" s="86">
+      <c r="I23" s="79">
         <f>H23*E23</f>
         <v>0</v>
       </c>
+      <c r="J23" s="120"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="I24" s="10" t="s">
+      <c r="A24" s="122"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="126"/>
+      <c r="I24" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J24" s="11">
+      <c r="J24" s="127">
         <f>SUM(I20:I23)</f>
         <v>9200</v>
       </c>
     </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="125"/>
+      <c r="B25" s="126"/>
+      <c r="C25" s="126"/>
+      <c r="D25" s="126"/>
+      <c r="E25" s="126"/>
+      <c r="F25" s="126"/>
+      <c r="G25" s="126"/>
+      <c r="H25" s="126"/>
+      <c r="I25" s="126"/>
+      <c r="J25" s="120"/>
+    </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B26" s="103" t="s">
+      <c r="A26" s="125"/>
+      <c r="B26" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="103"/>
-      <c r="D26" s="103"/>
-      <c r="E26" s="13" cm="1">
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="129" cm="1">
         <f t="array" ref="E26">SUM((31)*(F2:F23))</f>
         <v>270010</v>
       </c>
+      <c r="F26" s="126"/>
+      <c r="G26" s="126"/>
+      <c r="H26" s="126"/>
+      <c r="I26" s="126"/>
+      <c r="J26" s="120"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="89"/>
-      <c r="B27" s="102" t="s">
+      <c r="A27" s="131"/>
+      <c r="B27" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="102"/>
-      <c r="D27" s="102"/>
-      <c r="E27" s="87">
+      <c r="C27" s="132"/>
+      <c r="D27" s="132"/>
+      <c r="E27" s="133">
         <f>SUM(J24,J18,J11,J6)</f>
         <v>50165</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="103" t="s">
+      <c r="F27" s="126"/>
+      <c r="G27" s="126"/>
+      <c r="H27" s="126"/>
+      <c r="I27" s="126"/>
+      <c r="J27" s="120"/>
+    </row>
+    <row r="28" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="134"/>
+      <c r="B28" s="135" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="13">
+      <c r="C28" s="135"/>
+      <c r="D28" s="135"/>
+      <c r="E28" s="136">
         <f>E26+E27</f>
         <v>320175</v>
       </c>
+      <c r="F28" s="130"/>
+      <c r="G28" s="130"/>
+      <c r="H28" s="130"/>
+      <c r="I28" s="130"/>
+      <c r="J28" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5139,8 +5267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84BC5521-4988-4D0D-A028-B369FE76398F}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E28" sqref="B26:E28"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -5158,651 +5286,713 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="J1" s="119"/>
     </row>
     <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18">
+      <c r="C2" s="10"/>
+      <c r="D2" s="11">
         <v>8</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="11">
         <f>D2*4</f>
         <v>32</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="12">
         <v>220</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="12">
         <f>F2/8</f>
         <v>27.5</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="12">
         <f>2*G2</f>
         <v>55</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2" s="13">
         <f>H2*E2</f>
         <v>1760</v>
       </c>
+      <c r="J2" s="120"/>
     </row>
     <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24">
+      <c r="C3" s="16"/>
+      <c r="D3" s="17">
         <v>8</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="17">
         <f t="shared" ref="E3:E5" si="0">D3*4</f>
         <v>32</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="18">
         <v>225</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="18">
         <f t="shared" ref="G3:G5" si="1">F3/8</f>
         <v>28.125</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="18">
         <f>2*G3</f>
         <v>56.25</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I3" s="19">
         <f>H3*E3</f>
         <v>1800</v>
       </c>
+      <c r="J3" s="120"/>
     </row>
     <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24">
+      <c r="C4" s="16"/>
+      <c r="D4" s="17">
         <v>8</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="17">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="18">
         <v>850</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="18">
         <f t="shared" si="1"/>
         <v>106.25</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="18">
         <f>2*G4</f>
         <v>212.5</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I4" s="19">
         <f>H4*E4</f>
         <v>6800</v>
       </c>
+      <c r="J4" s="120"/>
     </row>
     <row r="5" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="30">
+      <c r="C5" s="22"/>
+      <c r="D5" s="23">
         <v>5</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="23">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="24">
         <v>1200</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="24">
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="24">
         <f>2*G5</f>
         <v>300</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="25">
         <f>H5*E5</f>
         <v>6000</v>
       </c>
+      <c r="J5" s="120"/>
     </row>
     <row r="6" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="8" t="s">
+      <c r="A6" s="122"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="6">
         <f>SUM(I2:I5)</f>
         <v>16360</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="A7" s="122"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="123"/>
+      <c r="H7" s="123"/>
+      <c r="I7" s="123"/>
+      <c r="J7" s="120"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="36">
+      <c r="C8" s="28"/>
+      <c r="D8" s="29">
         <v>5</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="29">
         <f>D8*4</f>
         <v>20</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="30">
         <v>250</v>
       </c>
-      <c r="G8" s="37">
+      <c r="G8" s="30">
         <f>F8/8</f>
         <v>31.25</v>
       </c>
-      <c r="H8" s="37">
+      <c r="H8" s="30">
         <f>2*G8</f>
         <v>62.5</v>
       </c>
-      <c r="I8" s="38">
+      <c r="I8" s="31">
         <f>H8*E8</f>
         <v>1250</v>
       </c>
+      <c r="J8" s="120"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42">
+      <c r="C9" s="34"/>
+      <c r="D9" s="35">
         <v>5</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="35">
         <f t="shared" ref="E9:E10" si="2">D9*4</f>
         <v>20</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="36">
         <v>225</v>
       </c>
-      <c r="G9" s="43">
+      <c r="G9" s="36">
         <f t="shared" ref="G9:G10" si="3">F9/8</f>
         <v>28.125</v>
       </c>
-      <c r="H9" s="43">
+      <c r="H9" s="36">
         <f>2*G9</f>
         <v>56.25</v>
       </c>
-      <c r="I9" s="44">
+      <c r="I9" s="37">
         <f>H9*E9</f>
         <v>1125</v>
       </c>
+      <c r="J9" s="120"/>
     </row>
     <row r="10" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="48">
+      <c r="C10" s="40"/>
+      <c r="D10" s="41">
         <v>8</v>
       </c>
-      <c r="E10" s="48">
+      <c r="E10" s="41">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="F10" s="49">
+      <c r="F10" s="42">
         <v>850</v>
       </c>
-      <c r="G10" s="49">
+      <c r="G10" s="42">
         <f t="shared" si="3"/>
         <v>106.25</v>
       </c>
-      <c r="H10" s="49">
+      <c r="H10" s="42">
         <f>2*G10</f>
         <v>212.5</v>
       </c>
-      <c r="I10" s="50">
+      <c r="I10" s="43">
         <f>H10*E10</f>
         <v>6800</v>
       </c>
+      <c r="J10" s="120"/>
     </row>
     <row r="11" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="8" t="s">
+      <c r="A11" s="122"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="123"/>
+      <c r="H11" s="124"/>
+      <c r="I11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="6">
         <f>SUM(I8:I10)</f>
         <v>9175</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="A12" s="125"/>
+      <c r="B12" s="126"/>
+      <c r="C12" s="126"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="124"/>
+      <c r="G12" s="124"/>
+      <c r="H12" s="124"/>
+      <c r="I12" s="126"/>
+      <c r="J12" s="120"/>
     </row>
     <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="54">
+      <c r="C13" s="46"/>
+      <c r="D13" s="47">
         <v>6</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="47">
         <f>D13*4</f>
         <v>24</v>
       </c>
-      <c r="F13" s="55">
+      <c r="F13" s="48">
         <v>220</v>
       </c>
-      <c r="G13" s="55">
+      <c r="G13" s="48">
         <f>F13/8</f>
         <v>27.5</v>
       </c>
-      <c r="H13" s="55">
+      <c r="H13" s="48">
         <f>2*G13</f>
         <v>55</v>
       </c>
-      <c r="I13" s="56">
+      <c r="I13" s="49">
         <f>H13*E13</f>
         <v>1320</v>
       </c>
+      <c r="J13" s="120"/>
     </row>
     <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="59"/>
-      <c r="D14" s="60">
+      <c r="C14" s="52"/>
+      <c r="D14" s="53">
         <v>6</v>
       </c>
-      <c r="E14" s="60">
+      <c r="E14" s="53">
         <f t="shared" ref="E14:E17" si="4">D14*4</f>
         <v>24</v>
       </c>
-      <c r="F14" s="61">
+      <c r="F14" s="54">
         <v>250</v>
       </c>
-      <c r="G14" s="61">
+      <c r="G14" s="54">
         <f t="shared" ref="G14:G17" si="5">F14/8</f>
         <v>31.25</v>
       </c>
-      <c r="H14" s="61">
+      <c r="H14" s="54">
         <f>2*G14</f>
         <v>62.5</v>
       </c>
-      <c r="I14" s="62">
+      <c r="I14" s="55">
         <f>H14*E14</f>
         <v>1500</v>
       </c>
+      <c r="J14" s="120"/>
     </row>
     <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="60">
+      <c r="C15" s="52"/>
+      <c r="D15" s="53">
         <v>6</v>
       </c>
-      <c r="E15" s="60">
+      <c r="E15" s="53">
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="F15" s="61">
+      <c r="F15" s="54">
         <v>300</v>
       </c>
-      <c r="G15" s="61">
+      <c r="G15" s="54">
         <f t="shared" si="5"/>
         <v>37.5</v>
       </c>
-      <c r="H15" s="61">
+      <c r="H15" s="54">
         <f>2*G15</f>
         <v>75</v>
       </c>
-      <c r="I15" s="62">
+      <c r="I15" s="55">
         <f>H15*E15</f>
         <v>1800</v>
       </c>
+      <c r="J15" s="120"/>
     </row>
     <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="60">
+      <c r="C16" s="52"/>
+      <c r="D16" s="53">
         <v>5</v>
       </c>
-      <c r="E16" s="60">
+      <c r="E16" s="53">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="F16" s="61">
+      <c r="F16" s="54">
         <v>750</v>
       </c>
-      <c r="G16" s="61">
+      <c r="G16" s="54">
         <f t="shared" si="5"/>
         <v>93.75</v>
       </c>
-      <c r="H16" s="61">
+      <c r="H16" s="54">
         <f>2*G16</f>
         <v>187.5</v>
       </c>
-      <c r="I16" s="62">
+      <c r="I16" s="55">
         <f>H16*E16</f>
         <v>3750</v>
       </c>
+      <c r="J16" s="120"/>
     </row>
     <row r="17" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="65"/>
-      <c r="D17" s="66">
+      <c r="C17" s="58"/>
+      <c r="D17" s="59">
         <v>1</v>
       </c>
-      <c r="E17" s="66">
+      <c r="E17" s="59">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="F17" s="67">
+      <c r="F17" s="60">
         <v>1600</v>
       </c>
-      <c r="G17" s="67">
+      <c r="G17" s="60">
         <f t="shared" si="5"/>
         <v>200</v>
       </c>
-      <c r="H17" s="67">
+      <c r="H17" s="60">
         <f>2*G17</f>
         <v>400</v>
       </c>
-      <c r="I17" s="68">
+      <c r="I17" s="61">
         <f>H17*E17</f>
         <v>1600</v>
       </c>
+      <c r="J17" s="120"/>
     </row>
     <row r="18" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="8" t="s">
+      <c r="A18" s="122"/>
+      <c r="B18" s="80"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="123"/>
+      <c r="G18" s="123"/>
+      <c r="H18" s="124"/>
+      <c r="I18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="6">
         <f>SUM(I13:I17)</f>
         <v>9970</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="A19" s="125"/>
+      <c r="B19" s="126"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="126"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="124"/>
+      <c r="H19" s="124"/>
+      <c r="I19" s="126"/>
+      <c r="J19" s="120"/>
     </row>
     <row r="20" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="70" t="s">
+      <c r="B20" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="71"/>
-      <c r="D20" s="72">
+      <c r="C20" s="64"/>
+      <c r="D20" s="65">
         <v>10</v>
       </c>
-      <c r="E20" s="72">
+      <c r="E20" s="65">
         <f>D20*4</f>
         <v>40</v>
       </c>
-      <c r="F20" s="73">
+      <c r="F20" s="66">
         <v>220</v>
       </c>
-      <c r="G20" s="73">
+      <c r="G20" s="66">
         <f>F20/8</f>
         <v>27.5</v>
       </c>
-      <c r="H20" s="73">
+      <c r="H20" s="66">
         <f>2*G20</f>
         <v>55</v>
       </c>
-      <c r="I20" s="74">
+      <c r="I20" s="67">
         <f>H20*E20</f>
         <v>2200</v>
       </c>
+      <c r="J20" s="120"/>
     </row>
     <row r="21" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="76" t="s">
+      <c r="B21" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="77"/>
-      <c r="D21" s="78">
+      <c r="C21" s="70"/>
+      <c r="D21" s="71">
         <v>10</v>
       </c>
-      <c r="E21" s="78">
+      <c r="E21" s="71">
         <f t="shared" ref="E21:E23" si="6">D21*4</f>
         <v>40</v>
       </c>
-      <c r="F21" s="79">
+      <c r="F21" s="72">
         <v>300</v>
       </c>
-      <c r="G21" s="79">
+      <c r="G21" s="72">
         <f t="shared" ref="G21:G23" si="7">F21/8</f>
         <v>37.5</v>
       </c>
-      <c r="H21" s="79">
+      <c r="H21" s="72">
         <f>2*G21</f>
         <v>75</v>
       </c>
-      <c r="I21" s="80">
+      <c r="I21" s="73">
         <f>H21*E21</f>
         <v>3000</v>
       </c>
+      <c r="J21" s="120"/>
     </row>
     <row r="22" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="75" t="s">
+      <c r="A22" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="76" t="s">
+      <c r="B22" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="77"/>
-      <c r="D22" s="78">
+      <c r="C22" s="70"/>
+      <c r="D22" s="71">
         <v>10</v>
       </c>
-      <c r="E22" s="78">
+      <c r="E22" s="71">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="F22" s="79">
+      <c r="F22" s="72">
         <v>400</v>
       </c>
-      <c r="G22" s="79">
+      <c r="G22" s="72">
         <f t="shared" si="7"/>
         <v>50</v>
       </c>
-      <c r="H22" s="79">
+      <c r="H22" s="72">
         <f>2*G22</f>
         <v>100</v>
       </c>
-      <c r="I22" s="80">
+      <c r="I22" s="73">
         <f>H22*E22</f>
         <v>4000</v>
       </c>
+      <c r="J22" s="120"/>
     </row>
     <row r="23" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="81" t="s">
+      <c r="A23" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="82" t="s">
+      <c r="B23" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="83"/>
-      <c r="D23" s="84">
+      <c r="C23" s="76"/>
+      <c r="D23" s="77">
         <v>3</v>
       </c>
-      <c r="E23" s="84">
+      <c r="E23" s="77">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
-      <c r="F23" s="85">
+      <c r="F23" s="78">
         <v>850</v>
       </c>
-      <c r="G23" s="85">
+      <c r="G23" s="78">
         <f t="shared" si="7"/>
         <v>106.25</v>
       </c>
-      <c r="H23" s="85">
+      <c r="H23" s="78">
         <f>2*G23</f>
         <v>212.5</v>
       </c>
-      <c r="I23" s="86">
+      <c r="I23" s="79">
         <f>H23*E23</f>
         <v>2550</v>
       </c>
+      <c r="J23" s="120"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="I24" s="10" t="s">
+      <c r="A24" s="122"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="126"/>
+      <c r="I24" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J24" s="11">
+      <c r="J24" s="127">
         <f>SUM(I20:I23)</f>
         <v>11750</v>
       </c>
     </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="125"/>
+      <c r="B25" s="126"/>
+      <c r="C25" s="126"/>
+      <c r="D25" s="126"/>
+      <c r="E25" s="126"/>
+      <c r="F25" s="126"/>
+      <c r="G25" s="126"/>
+      <c r="H25" s="126"/>
+      <c r="I25" s="126"/>
+      <c r="J25" s="120"/>
+    </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B26" s="103" t="s">
+      <c r="A26" s="125"/>
+      <c r="B26" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="103"/>
-      <c r="D26" s="103"/>
-      <c r="E26" s="13" cm="1">
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="129" cm="1">
         <f t="array" ref="E26">SUM((28)*(F2:F23))</f>
         <v>243880</v>
       </c>
+      <c r="F26" s="126"/>
+      <c r="G26" s="126"/>
+      <c r="H26" s="126"/>
+      <c r="I26" s="126"/>
+      <c r="J26" s="120"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="89"/>
-      <c r="B27" s="102" t="s">
+      <c r="A27" s="131"/>
+      <c r="B27" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="102"/>
-      <c r="D27" s="102"/>
-      <c r="E27" s="87">
+      <c r="C27" s="132"/>
+      <c r="D27" s="132"/>
+      <c r="E27" s="133">
         <f>SUM(J24,J18,J11,J6)</f>
         <v>47255</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="103" t="s">
+      <c r="F27" s="126"/>
+      <c r="G27" s="126"/>
+      <c r="H27" s="126"/>
+      <c r="I27" s="126"/>
+      <c r="J27" s="120"/>
+    </row>
+    <row r="28" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="134"/>
+      <c r="B28" s="135" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="13">
+      <c r="C28" s="135"/>
+      <c r="D28" s="135"/>
+      <c r="E28" s="136">
         <f>E26+E27</f>
         <v>291135</v>
       </c>
+      <c r="F28" s="130"/>
+      <c r="G28" s="130"/>
+      <c r="H28" s="130"/>
+      <c r="I28" s="130"/>
+      <c r="J28" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5819,8 +6009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726DBE1C-F047-4F19-9C72-4C60A2C4AD9C}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -5838,713 +6028,777 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="J1" s="119"/>
     </row>
     <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18">
+      <c r="C2" s="10"/>
+      <c r="D2" s="11">
         <v>7</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="11">
         <f>D2*4</f>
         <v>28</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="12">
         <v>220</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="12">
         <f>F2/8</f>
         <v>27.5</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="12">
         <f>2*G2</f>
         <v>55</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2" s="13">
         <f>H2*E2</f>
         <v>1540</v>
       </c>
+      <c r="J2" s="120"/>
     </row>
     <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24">
+      <c r="C3" s="16"/>
+      <c r="D3" s="17">
         <v>7</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="17">
         <f t="shared" ref="E3" si="0">D3*4</f>
         <v>28</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="18">
         <v>225</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="18">
         <f t="shared" ref="G3" si="1">F3/8</f>
         <v>28.125</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="18">
         <f>2*G3</f>
         <v>56.25</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I3" s="19">
         <f>H3*E3</f>
         <v>1575</v>
       </c>
+      <c r="J3" s="120"/>
     </row>
     <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24">
+      <c r="C4" s="16"/>
+      <c r="D4" s="17">
         <v>7</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="17">
         <f t="shared" ref="E4:E6" si="2">D4*4</f>
         <v>28</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="18">
         <v>225</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="18">
         <f t="shared" ref="G4:G6" si="3">F4/8</f>
         <v>28.125</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="18">
         <f>2*G4</f>
         <v>56.25</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I4" s="19">
         <f>H4*E4</f>
         <v>1575</v>
       </c>
+      <c r="J4" s="120"/>
     </row>
     <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24">
+      <c r="C5" s="16"/>
+      <c r="D5" s="17">
         <v>7</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="17">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="18">
         <v>850</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="18">
         <f t="shared" si="3"/>
         <v>106.25</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="18">
         <f>2*G5</f>
         <v>212.5</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="19">
         <f>H5*E5</f>
         <v>5950</v>
       </c>
+      <c r="J5" s="120"/>
     </row>
     <row r="6" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="30">
+      <c r="C6" s="22"/>
+      <c r="D6" s="23">
         <v>7</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="23">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="24">
         <v>1200</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="24">
         <f t="shared" si="3"/>
         <v>150</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="24">
         <f>2*G6</f>
         <v>300</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="25">
         <f>H6*E6</f>
         <v>8400</v>
       </c>
+      <c r="J6" s="120"/>
     </row>
     <row r="7" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="8" t="s">
+      <c r="A7" s="122"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="123"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="6">
         <f>SUM(I2:I6)</f>
         <v>19040</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="A8" s="122"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="123"/>
+      <c r="H8" s="123"/>
+      <c r="I8" s="123"/>
+      <c r="J8" s="120"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="36">
+      <c r="C9" s="28"/>
+      <c r="D9" s="29">
         <v>8</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="29">
         <f>D9*4</f>
         <v>32</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="30">
         <v>250</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="30">
         <f>F9/8</f>
         <v>31.25</v>
       </c>
-      <c r="H9" s="37">
+      <c r="H9" s="30">
         <f>2*G9</f>
         <v>62.5</v>
       </c>
-      <c r="I9" s="38">
+      <c r="I9" s="31">
         <f>H9*E9</f>
         <v>2000</v>
       </c>
+      <c r="J9" s="120"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="42">
+      <c r="C10" s="34"/>
+      <c r="D10" s="35">
         <v>8</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="35">
         <f t="shared" ref="E10:E11" si="4">D10*4</f>
         <v>32</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="36">
         <v>225</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="36">
         <f t="shared" ref="G10:G11" si="5">F10/8</f>
         <v>28.125</v>
       </c>
-      <c r="H10" s="43">
+      <c r="H10" s="36">
         <f>2*G10</f>
         <v>56.25</v>
       </c>
-      <c r="I10" s="44">
+      <c r="I10" s="37">
         <f>H10*E10</f>
         <v>1800</v>
       </c>
+      <c r="J10" s="120"/>
     </row>
     <row r="11" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="48">
+      <c r="C11" s="40"/>
+      <c r="D11" s="41">
         <v>7</v>
       </c>
-      <c r="E11" s="48">
+      <c r="E11" s="41">
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="F11" s="49">
+      <c r="F11" s="42">
         <v>850</v>
       </c>
-      <c r="G11" s="49">
+      <c r="G11" s="42">
         <f t="shared" si="5"/>
         <v>106.25</v>
       </c>
-      <c r="H11" s="49">
+      <c r="H11" s="42">
         <f>2*G11</f>
         <v>212.5</v>
       </c>
-      <c r="I11" s="50">
+      <c r="I11" s="43">
         <f>H11*E11</f>
         <v>5950</v>
       </c>
+      <c r="J11" s="120"/>
     </row>
     <row r="12" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="8" t="s">
+      <c r="A12" s="122"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="124"/>
+      <c r="I12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="6">
         <f>SUM(I9:I11)</f>
         <v>9750</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="A13" s="125"/>
+      <c r="B13" s="126"/>
+      <c r="C13" s="126"/>
+      <c r="D13" s="126"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="124"/>
+      <c r="H13" s="124"/>
+      <c r="I13" s="126"/>
+      <c r="J13" s="120"/>
     </row>
     <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="54">
+      <c r="C14" s="46"/>
+      <c r="D14" s="47">
         <v>7</v>
       </c>
-      <c r="E14" s="54">
+      <c r="E14" s="47">
         <f>D14*4</f>
         <v>28</v>
       </c>
-      <c r="F14" s="55">
+      <c r="F14" s="48">
         <v>220</v>
       </c>
-      <c r="G14" s="55">
+      <c r="G14" s="48">
         <f>F14/8</f>
         <v>27.5</v>
       </c>
-      <c r="H14" s="55">
+      <c r="H14" s="48">
         <f>2*G14</f>
         <v>55</v>
       </c>
-      <c r="I14" s="56">
+      <c r="I14" s="49">
         <f>H14*E14</f>
         <v>1540</v>
       </c>
+      <c r="J14" s="120"/>
     </row>
     <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="60">
+      <c r="C15" s="52"/>
+      <c r="D15" s="53">
         <v>7</v>
       </c>
-      <c r="E15" s="60">
+      <c r="E15" s="53">
         <f t="shared" ref="E15:E18" si="6">D15*4</f>
         <v>28</v>
       </c>
-      <c r="F15" s="61">
+      <c r="F15" s="54">
         <v>250</v>
       </c>
-      <c r="G15" s="61">
+      <c r="G15" s="54">
         <f t="shared" ref="G15:G18" si="7">F15/8</f>
         <v>31.25</v>
       </c>
-      <c r="H15" s="61">
+      <c r="H15" s="54">
         <f>2*G15</f>
         <v>62.5</v>
       </c>
-      <c r="I15" s="62">
+      <c r="I15" s="55">
         <f>H15*E15</f>
         <v>1750</v>
       </c>
+      <c r="J15" s="120"/>
     </row>
     <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="60">
+      <c r="C16" s="52"/>
+      <c r="D16" s="53">
         <v>7</v>
       </c>
-      <c r="E16" s="60">
+      <c r="E16" s="53">
         <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="F16" s="61">
+      <c r="F16" s="54">
         <v>300</v>
       </c>
-      <c r="G16" s="61">
+      <c r="G16" s="54">
         <f t="shared" si="7"/>
         <v>37.5</v>
       </c>
-      <c r="H16" s="61">
+      <c r="H16" s="54">
         <f>2*G16</f>
         <v>75</v>
       </c>
-      <c r="I16" s="62">
+      <c r="I16" s="55">
         <f>H16*E16</f>
         <v>2100</v>
       </c>
+      <c r="J16" s="120"/>
     </row>
     <row r="17" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="60">
+      <c r="C17" s="52"/>
+      <c r="D17" s="53">
         <v>7</v>
       </c>
-      <c r="E17" s="60">
+      <c r="E17" s="53">
         <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="F17" s="61">
+      <c r="F17" s="54">
         <v>750</v>
       </c>
-      <c r="G17" s="61">
+      <c r="G17" s="54">
         <f t="shared" si="7"/>
         <v>93.75</v>
       </c>
-      <c r="H17" s="61">
+      <c r="H17" s="54">
         <f>2*G17</f>
         <v>187.5</v>
       </c>
-      <c r="I17" s="62">
+      <c r="I17" s="55">
         <f>H17*E17</f>
         <v>5250</v>
       </c>
+      <c r="J17" s="120"/>
     </row>
     <row r="18" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="65"/>
-      <c r="D18" s="66">
+      <c r="C18" s="58"/>
+      <c r="D18" s="59">
         <v>3</v>
       </c>
-      <c r="E18" s="66">
+      <c r="E18" s="59">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
-      <c r="F18" s="67">
+      <c r="F18" s="60">
         <v>1600</v>
       </c>
-      <c r="G18" s="67">
+      <c r="G18" s="60">
         <f t="shared" si="7"/>
         <v>200</v>
       </c>
-      <c r="H18" s="67">
+      <c r="H18" s="60">
         <f>2*G18</f>
         <v>400</v>
       </c>
-      <c r="I18" s="68">
+      <c r="I18" s="61">
         <f>H18*E18</f>
         <v>4800</v>
       </c>
+      <c r="J18" s="120"/>
     </row>
     <row r="19" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="8" t="s">
+      <c r="A19" s="122"/>
+      <c r="B19" s="80"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="123"/>
+      <c r="G19" s="123"/>
+      <c r="H19" s="124"/>
+      <c r="I19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="6">
         <f>SUM(I14:I18)</f>
         <v>15440</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
+      <c r="A20" s="125"/>
+      <c r="B20" s="126"/>
+      <c r="C20" s="126"/>
+      <c r="D20" s="126"/>
+      <c r="E20" s="126"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="124"/>
+      <c r="H20" s="124"/>
+      <c r="I20" s="126"/>
+      <c r="J20" s="120"/>
     </row>
     <row r="21" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="69" t="s">
+      <c r="A21" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="71"/>
-      <c r="D21" s="72">
+      <c r="C21" s="64"/>
+      <c r="D21" s="65">
         <v>8</v>
       </c>
-      <c r="E21" s="72">
+      <c r="E21" s="65">
         <f>D21*4</f>
         <v>32</v>
       </c>
-      <c r="F21" s="73">
+      <c r="F21" s="66">
         <v>220</v>
       </c>
-      <c r="G21" s="73">
+      <c r="G21" s="66">
         <f>F21/8</f>
         <v>27.5</v>
       </c>
-      <c r="H21" s="73">
+      <c r="H21" s="66">
         <f>2*G21</f>
         <v>55</v>
       </c>
-      <c r="I21" s="74">
+      <c r="I21" s="67">
         <f>H21*E21</f>
         <v>1760</v>
       </c>
+      <c r="J21" s="120"/>
     </row>
     <row r="22" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="75" t="s">
+      <c r="A22" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="76" t="s">
+      <c r="B22" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="77"/>
-      <c r="D22" s="78">
+      <c r="C22" s="70"/>
+      <c r="D22" s="71">
         <v>8</v>
       </c>
-      <c r="E22" s="78">
+      <c r="E22" s="71">
         <f t="shared" ref="E22" si="8">D22*4</f>
         <v>32</v>
       </c>
-      <c r="F22" s="79">
+      <c r="F22" s="72">
         <v>300</v>
       </c>
-      <c r="G22" s="79">
+      <c r="G22" s="72">
         <f t="shared" ref="G22" si="9">F22/8</f>
         <v>37.5</v>
       </c>
-      <c r="H22" s="79">
+      <c r="H22" s="72">
         <f>2*G22</f>
         <v>75</v>
       </c>
-      <c r="I22" s="80">
+      <c r="I22" s="73">
         <f>H22*E22</f>
         <v>2400</v>
       </c>
+      <c r="J22" s="120"/>
     </row>
     <row r="23" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="75" t="s">
+      <c r="A23" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="77"/>
-      <c r="D23" s="78">
+      <c r="C23" s="70"/>
+      <c r="D23" s="71">
         <v>12</v>
       </c>
-      <c r="E23" s="78">
+      <c r="E23" s="71">
         <f t="shared" ref="E23:E25" si="10">D23*4</f>
         <v>48</v>
       </c>
-      <c r="F23" s="79">
+      <c r="F23" s="72">
         <v>300</v>
       </c>
-      <c r="G23" s="79">
+      <c r="G23" s="72">
         <f t="shared" ref="G23:G25" si="11">F23/8</f>
         <v>37.5</v>
       </c>
-      <c r="H23" s="79">
+      <c r="H23" s="72">
         <f>2*G23</f>
         <v>75</v>
       </c>
-      <c r="I23" s="80">
+      <c r="I23" s="73">
         <f>H23*E23</f>
         <v>3600</v>
       </c>
+      <c r="J23" s="120"/>
     </row>
     <row r="24" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="75" t="s">
+      <c r="A24" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="76" t="s">
+      <c r="B24" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="77"/>
-      <c r="D24" s="78">
+      <c r="C24" s="70"/>
+      <c r="D24" s="71">
         <v>12</v>
       </c>
-      <c r="E24" s="78">
+      <c r="E24" s="71">
         <f t="shared" si="10"/>
         <v>48</v>
       </c>
-      <c r="F24" s="79">
+      <c r="F24" s="72">
         <v>400</v>
       </c>
-      <c r="G24" s="79">
+      <c r="G24" s="72">
         <f t="shared" si="11"/>
         <v>50</v>
       </c>
-      <c r="H24" s="79">
+      <c r="H24" s="72">
         <f>2*G24</f>
         <v>100</v>
       </c>
-      <c r="I24" s="80">
+      <c r="I24" s="73">
         <f>H24*E24</f>
         <v>4800</v>
       </c>
+      <c r="J24" s="120"/>
     </row>
     <row r="25" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="81" t="s">
+      <c r="A25" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="82" t="s">
+      <c r="B25" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="83"/>
-      <c r="D25" s="84">
+      <c r="C25" s="76"/>
+      <c r="D25" s="77">
         <v>5</v>
       </c>
-      <c r="E25" s="84">
+      <c r="E25" s="77">
         <f t="shared" si="10"/>
         <v>20</v>
       </c>
-      <c r="F25" s="85">
+      <c r="F25" s="78">
         <v>850</v>
       </c>
-      <c r="G25" s="85">
+      <c r="G25" s="78">
         <f t="shared" si="11"/>
         <v>106.25</v>
       </c>
-      <c r="H25" s="85">
+      <c r="H25" s="78">
         <f>2*G25</f>
         <v>212.5</v>
       </c>
-      <c r="I25" s="86">
+      <c r="I25" s="79">
         <f>H25*E25</f>
         <v>4250</v>
       </c>
+      <c r="J25" s="120"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="I26" s="10" t="s">
+      <c r="A26" s="122"/>
+      <c r="B26" s="80"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="81"/>
+      <c r="G26" s="81"/>
+      <c r="H26" s="126"/>
+      <c r="I26" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J26" s="11">
+      <c r="J26" s="127">
         <f>SUM(I21:I25)</f>
         <v>16810</v>
       </c>
     </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="125"/>
+      <c r="B27" s="126"/>
+      <c r="C27" s="126"/>
+      <c r="D27" s="126"/>
+      <c r="E27" s="126"/>
+      <c r="F27" s="126"/>
+      <c r="G27" s="126"/>
+      <c r="H27" s="126"/>
+      <c r="I27" s="126"/>
+      <c r="J27" s="120"/>
+    </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="103" t="s">
+      <c r="A28" s="125"/>
+      <c r="B28" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="13" cm="1">
+      <c r="C28" s="128"/>
+      <c r="D28" s="128"/>
+      <c r="E28" s="129" cm="1">
         <f t="array" ref="E28">SUM((31)*(F2:F25))</f>
         <v>286285</v>
       </c>
+      <c r="F28" s="126"/>
+      <c r="G28" s="126"/>
+      <c r="H28" s="126"/>
+      <c r="I28" s="126"/>
+      <c r="J28" s="120"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="89"/>
-      <c r="B29" s="102" t="s">
+      <c r="A29" s="131"/>
+      <c r="B29" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="102"/>
-      <c r="D29" s="102"/>
-      <c r="E29" s="87">
+      <c r="C29" s="132"/>
+      <c r="D29" s="132"/>
+      <c r="E29" s="133">
         <f>SUM(J26,J19,J12,J7)</f>
         <v>61040</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="103" t="s">
+      <c r="F29" s="126"/>
+      <c r="G29" s="126"/>
+      <c r="H29" s="126"/>
+      <c r="I29" s="126"/>
+      <c r="J29" s="120"/>
+    </row>
+    <row r="30" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="134"/>
+      <c r="B30" s="135" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="103"/>
-      <c r="D30" s="103"/>
-      <c r="E30" s="13">
+      <c r="C30" s="135"/>
+      <c r="D30" s="135"/>
+      <c r="E30" s="136">
         <f>E28+E29</f>
         <v>347325</v>
       </c>
+      <c r="F30" s="130"/>
+      <c r="G30" s="130"/>
+      <c r="H30" s="130"/>
+      <c r="I30" s="130"/>
+      <c r="J30" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6561,8 +6815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8581AE50-5B11-446D-B899-0F87E4792975}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -6581,762 +6835,833 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="100" t="s">
+      <c r="C1" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100" t="s">
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="100" t="s">
+      <c r="I1" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="100" t="s">
+      <c r="J1" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="100" t="s">
+      <c r="K1" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="101" t="s">
+      <c r="L1" s="89" t="s">
         <v>6</v>
       </c>
+      <c r="M1" s="119"/>
     </row>
     <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18">
+      <c r="C2" s="10"/>
+      <c r="D2" s="11">
         <v>5</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="11">
         <v>3</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11">
         <f>SUM(D2:G2)</f>
         <v>8</v>
       </c>
-      <c r="I2" s="19">
+      <c r="I2" s="12">
         <v>225</v>
       </c>
-      <c r="J2" s="19">
+      <c r="J2" s="12">
         <f t="shared" ref="J2:J5" si="0">I2/8</f>
         <v>28.125</v>
       </c>
-      <c r="K2" s="19">
+      <c r="K2" s="12">
         <f>2*J2</f>
         <v>56.25</v>
       </c>
-      <c r="L2" s="20">
+      <c r="L2" s="13">
         <f>K2*H2</f>
         <v>450</v>
       </c>
+      <c r="M2" s="120"/>
     </row>
     <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24">
+      <c r="C3" s="16"/>
+      <c r="D3" s="17">
         <v>5</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="17">
         <v>3</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17">
         <f t="shared" ref="H3:H23" si="1">SUM(D3:G3)</f>
         <v>8</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="18">
         <v>225</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="18">
         <f t="shared" si="0"/>
         <v>28.125</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3" s="18">
         <f>2*J3</f>
         <v>56.25</v>
       </c>
-      <c r="L3" s="26">
+      <c r="L3" s="19">
         <f>K3*H3</f>
         <v>450</v>
       </c>
+      <c r="M3" s="120"/>
     </row>
     <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24">
+      <c r="C4" s="16"/>
+      <c r="D4" s="17">
         <v>5</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="17">
         <v>3</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="18">
         <v>850</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="18">
         <f t="shared" si="0"/>
         <v>106.25</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="18">
         <f>2*J4</f>
         <v>212.5</v>
       </c>
-      <c r="L4" s="26">
+      <c r="L4" s="19">
         <f>K4*H4</f>
         <v>1700</v>
       </c>
+      <c r="M4" s="120"/>
     </row>
     <row r="5" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="30">
+      <c r="C5" s="22"/>
+      <c r="D5" s="23">
         <v>1</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="23">
         <v>0.3</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30">
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23">
         <f t="shared" si="1"/>
         <v>1.3</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="24">
         <v>1200</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="24">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="24">
         <f>2*J5</f>
         <v>300</v>
       </c>
-      <c r="L5" s="98">
+      <c r="L5" s="86">
         <f>K5*H5</f>
         <v>390</v>
       </c>
+      <c r="M5" s="120"/>
     </row>
     <row r="6" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="92"/>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="94"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="95" t="s">
+      <c r="A6" s="122"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="123"/>
+      <c r="J6" s="123"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="6">
         <f>SUM(L2:L5)</f>
         <v>2990</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="92"/>
-      <c r="B7" s="92"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
+      <c r="A7" s="122"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="123"/>
+      <c r="J7" s="123"/>
+      <c r="K7" s="123"/>
+      <c r="L7" s="123"/>
+      <c r="M7" s="120"/>
     </row>
     <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="36">
+      <c r="C8" s="28"/>
+      <c r="D8" s="29">
         <v>6</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="29">
         <v>5</v>
       </c>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36">
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I8" s="37">
+      <c r="I8" s="30">
         <v>250</v>
       </c>
-      <c r="J8" s="37">
+      <c r="J8" s="30">
         <f>I8/8</f>
         <v>31.25</v>
       </c>
-      <c r="K8" s="37">
+      <c r="K8" s="30">
         <f>2*J8</f>
         <v>62.5</v>
       </c>
-      <c r="L8" s="38">
+      <c r="L8" s="31">
         <f>K8*H8</f>
         <v>687.5</v>
       </c>
+      <c r="M8" s="120"/>
     </row>
     <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42">
+      <c r="C9" s="34"/>
+      <c r="D9" s="35">
         <v>4</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="35">
         <v>5</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42">
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I9" s="43">
+      <c r="I9" s="36">
         <v>225</v>
       </c>
-      <c r="J9" s="43">
+      <c r="J9" s="36">
         <f t="shared" ref="J9:J10" si="2">I9/8</f>
         <v>28.125</v>
       </c>
-      <c r="K9" s="43">
+      <c r="K9" s="36">
         <f>2*J9</f>
         <v>56.25</v>
       </c>
-      <c r="L9" s="44">
+      <c r="L9" s="37">
         <f>K9*H9</f>
         <v>506.25</v>
       </c>
+      <c r="M9" s="120"/>
     </row>
     <row r="10" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="48">
+      <c r="C10" s="40"/>
+      <c r="D10" s="41">
         <v>1</v>
       </c>
-      <c r="E10" s="48">
+      <c r="E10" s="41">
         <v>1</v>
       </c>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48">
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I10" s="49">
+      <c r="I10" s="42">
         <v>850</v>
       </c>
-      <c r="J10" s="49">
+      <c r="J10" s="42">
         <f t="shared" si="2"/>
         <v>106.25</v>
       </c>
-      <c r="K10" s="49">
+      <c r="K10" s="42">
         <f>2*J10</f>
         <v>212.5</v>
       </c>
-      <c r="L10" s="97">
+      <c r="L10" s="85">
         <f>K10*H10</f>
         <v>425</v>
       </c>
+      <c r="M10" s="120"/>
     </row>
     <row r="11" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="90"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="95" t="s">
+      <c r="A11" s="122"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="123"/>
+      <c r="J11" s="123"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M11" s="6">
         <f>SUM(L8:L10)</f>
         <v>1618.75</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G12" s="91"/>
-      <c r="H12" s="94"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
+      <c r="A12" s="125"/>
+      <c r="B12" s="126"/>
+      <c r="C12" s="126"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
+      <c r="G12" s="137"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="124"/>
+      <c r="J12" s="124"/>
+      <c r="K12" s="124"/>
+      <c r="L12" s="126"/>
+      <c r="M12" s="120"/>
     </row>
     <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="54">
+      <c r="C13" s="46"/>
+      <c r="D13" s="47">
         <v>4</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="47">
         <v>5</v>
       </c>
-      <c r="F13" s="54">
+      <c r="F13" s="47">
         <v>0</v>
       </c>
-      <c r="G13" s="54">
+      <c r="G13" s="47">
         <v>0</v>
       </c>
-      <c r="H13" s="54">
+      <c r="H13" s="47">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I13" s="55">
+      <c r="I13" s="48">
         <v>220</v>
       </c>
-      <c r="J13" s="55">
+      <c r="J13" s="48">
         <f>I13/8</f>
         <v>27.5</v>
       </c>
-      <c r="K13" s="55">
+      <c r="K13" s="48">
         <f>2*J13</f>
         <v>55</v>
       </c>
-      <c r="L13" s="56">
+      <c r="L13" s="49">
         <f>K13*H13</f>
         <v>495</v>
       </c>
+      <c r="M13" s="120"/>
     </row>
     <row r="14" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="59"/>
-      <c r="D14" s="60">
+      <c r="C14" s="52"/>
+      <c r="D14" s="53">
         <v>4</v>
       </c>
-      <c r="E14" s="60">
+      <c r="E14" s="53">
         <v>1</v>
       </c>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60">
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I14" s="61">
+      <c r="I14" s="54">
         <v>250</v>
       </c>
-      <c r="J14" s="61">
+      <c r="J14" s="54">
         <f t="shared" ref="J14:J17" si="3">I14/8</f>
         <v>31.25</v>
       </c>
-      <c r="K14" s="61">
+      <c r="K14" s="54">
         <f>2*J14</f>
         <v>62.5</v>
       </c>
-      <c r="L14" s="62">
+      <c r="L14" s="55">
         <f>K14*H14</f>
         <v>312.5</v>
       </c>
+      <c r="M14" s="120"/>
     </row>
     <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="60">
+      <c r="C15" s="52"/>
+      <c r="D15" s="53">
         <v>4</v>
       </c>
-      <c r="E15" s="60">
+      <c r="E15" s="53">
         <v>5</v>
       </c>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60">
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I15" s="61">
+      <c r="I15" s="54">
         <v>300</v>
       </c>
-      <c r="J15" s="61">
+      <c r="J15" s="54">
         <f t="shared" si="3"/>
         <v>37.5</v>
       </c>
-      <c r="K15" s="61">
+      <c r="K15" s="54">
         <f>2*J15</f>
         <v>75</v>
       </c>
-      <c r="L15" s="62">
+      <c r="L15" s="55">
         <f>K15*H15</f>
         <v>675</v>
       </c>
+      <c r="M15" s="120"/>
     </row>
     <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="60">
+      <c r="C16" s="52"/>
+      <c r="D16" s="53">
         <v>4</v>
       </c>
-      <c r="E16" s="60">
+      <c r="E16" s="53">
         <v>5</v>
       </c>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60">
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I16" s="61">
+      <c r="I16" s="54">
         <v>750</v>
       </c>
-      <c r="J16" s="61">
+      <c r="J16" s="54">
         <f t="shared" si="3"/>
         <v>93.75</v>
       </c>
-      <c r="K16" s="61">
+      <c r="K16" s="54">
         <f>2*J16</f>
         <v>187.5</v>
       </c>
-      <c r="L16" s="62">
+      <c r="L16" s="55">
         <f>K16*H16</f>
         <v>1687.5</v>
       </c>
+      <c r="M16" s="120"/>
     </row>
     <row r="17" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="65"/>
-      <c r="D17" s="66">
+      <c r="C17" s="58"/>
+      <c r="D17" s="59">
         <v>2</v>
       </c>
-      <c r="E17" s="66">
+      <c r="E17" s="59">
         <v>5</v>
       </c>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66">
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I17" s="67">
+      <c r="I17" s="60">
         <v>1600</v>
       </c>
-      <c r="J17" s="67">
+      <c r="J17" s="60">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
-      <c r="K17" s="67">
+      <c r="K17" s="60">
         <f>2*J17</f>
         <v>400</v>
       </c>
-      <c r="L17" s="96">
+      <c r="L17" s="84">
         <f>K17*H17</f>
         <v>2800</v>
       </c>
+      <c r="M17" s="120"/>
     </row>
     <row r="18" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="94"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="95" t="s">
+      <c r="A18" s="122"/>
+      <c r="B18" s="80"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="123"/>
+      <c r="J18" s="123"/>
+      <c r="K18" s="124"/>
+      <c r="L18" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="M18" s="9">
+      <c r="M18" s="6">
         <f>SUM(L13:L17)</f>
         <v>5970</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H19" s="94"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
+      <c r="A19" s="125"/>
+      <c r="B19" s="126"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="126"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="126"/>
+      <c r="G19" s="126"/>
+      <c r="H19" s="82"/>
+      <c r="I19" s="124"/>
+      <c r="J19" s="124"/>
+      <c r="K19" s="124"/>
+      <c r="L19" s="126"/>
+      <c r="M19" s="120"/>
     </row>
     <row r="20" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="70" t="s">
+      <c r="B20" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="71"/>
-      <c r="D20" s="72">
+      <c r="C20" s="64"/>
+      <c r="D20" s="65">
         <v>3</v>
       </c>
-      <c r="E20" s="72">
+      <c r="E20" s="65">
         <v>4</v>
       </c>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
-      <c r="H20" s="72">
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I20" s="73">
+      <c r="I20" s="66">
         <v>220</v>
       </c>
-      <c r="J20" s="73">
+      <c r="J20" s="66">
         <f>I20/8</f>
         <v>27.5</v>
       </c>
-      <c r="K20" s="73">
+      <c r="K20" s="66">
         <f>2*J20</f>
         <v>55</v>
       </c>
-      <c r="L20" s="74">
+      <c r="L20" s="67">
         <f>K20*H20</f>
         <v>385</v>
       </c>
+      <c r="M20" s="120"/>
     </row>
     <row r="21" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="76" t="s">
+      <c r="B21" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="77"/>
-      <c r="D21" s="78">
+      <c r="C21" s="70"/>
+      <c r="D21" s="71">
         <v>3</v>
       </c>
-      <c r="E21" s="78">
+      <c r="E21" s="71">
         <v>4</v>
       </c>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78">
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I21" s="79">
+      <c r="I21" s="72">
         <v>300</v>
       </c>
-      <c r="J21" s="79">
+      <c r="J21" s="72">
         <f t="shared" ref="J21:J23" si="4">I21/8</f>
         <v>37.5</v>
       </c>
-      <c r="K21" s="79">
+      <c r="K21" s="72">
         <f>2*J21</f>
         <v>75</v>
       </c>
-      <c r="L21" s="80">
+      <c r="L21" s="73">
         <f>K21*H21</f>
         <v>525</v>
       </c>
+      <c r="M21" s="120"/>
     </row>
     <row r="22" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="75" t="s">
+      <c r="A22" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="76" t="s">
+      <c r="B22" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="77"/>
-      <c r="D22" s="78">
+      <c r="C22" s="70"/>
+      <c r="D22" s="71">
         <v>4</v>
       </c>
-      <c r="E22" s="78">
+      <c r="E22" s="71">
         <v>3</v>
       </c>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78">
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I22" s="79">
+      <c r="I22" s="72">
         <v>400</v>
       </c>
-      <c r="J22" s="79">
+      <c r="J22" s="72">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
-      <c r="K22" s="79">
+      <c r="K22" s="72">
         <f>2*J22</f>
         <v>100</v>
       </c>
-      <c r="L22" s="80">
+      <c r="L22" s="73">
         <f>K22*H22</f>
         <v>700</v>
       </c>
+      <c r="M22" s="120"/>
     </row>
     <row r="23" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="81" t="s">
+      <c r="A23" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="82" t="s">
+      <c r="B23" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="83"/>
-      <c r="D23" s="84">
+      <c r="C23" s="76"/>
+      <c r="D23" s="77">
         <v>2</v>
       </c>
-      <c r="E23" s="84">
+      <c r="E23" s="77">
         <v>1</v>
       </c>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84">
+      <c r="F23" s="77"/>
+      <c r="G23" s="77"/>
+      <c r="H23" s="77">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I23" s="85">
+      <c r="I23" s="78">
         <v>850</v>
       </c>
-      <c r="J23" s="85">
+      <c r="J23" s="78">
         <f t="shared" si="4"/>
         <v>106.25</v>
       </c>
-      <c r="K23" s="85">
+      <c r="K23" s="78">
         <f>2*J23</f>
         <v>212.5</v>
       </c>
-      <c r="L23" s="86">
+      <c r="L23" s="79">
         <f>K23*H23</f>
         <v>637.5</v>
       </c>
+      <c r="M23" s="120"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="L24" s="10" t="s">
+      <c r="A24" s="122"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="81"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="126"/>
+      <c r="L24" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="M24" s="11">
+      <c r="M24" s="127">
         <f>SUM(L20:L23)</f>
         <v>2247.5</v>
       </c>
     </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="125"/>
+      <c r="B25" s="126"/>
+      <c r="C25" s="126"/>
+      <c r="D25" s="126"/>
+      <c r="E25" s="126"/>
+      <c r="F25" s="126"/>
+      <c r="G25" s="126"/>
+      <c r="H25" s="126"/>
+      <c r="I25" s="126"/>
+      <c r="J25" s="126"/>
+      <c r="K25" s="126"/>
+      <c r="L25" s="126"/>
+      <c r="M25" s="120"/>
+    </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="103" t="s">
+      <c r="A26" s="125"/>
+      <c r="B26" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="103"/>
-      <c r="D26" s="103"/>
-      <c r="E26" s="13" cm="1">
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="129" cm="1">
         <f t="array" ref="E26">SUM((30)*(I2:I23))</f>
         <v>261450</v>
       </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
+      <c r="F26" s="138"/>
+      <c r="G26" s="138"/>
+      <c r="H26" s="126"/>
+      <c r="I26" s="126"/>
+      <c r="J26" s="126"/>
+      <c r="K26" s="126"/>
+      <c r="L26" s="126"/>
+      <c r="M26" s="120"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="89"/>
-      <c r="B27" s="102" t="s">
+      <c r="A27" s="131"/>
+      <c r="B27" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="102"/>
-      <c r="D27" s="102"/>
-      <c r="E27" s="87">
+      <c r="C27" s="132"/>
+      <c r="D27" s="132"/>
+      <c r="E27" s="133">
         <f>SUM(M24,M18,M11,M6)</f>
         <v>12826.25</v>
       </c>
-      <c r="F27" s="88"/>
-      <c r="G27" s="88"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="103" t="s">
+      <c r="F27" s="139"/>
+      <c r="G27" s="139"/>
+      <c r="H27" s="126"/>
+      <c r="I27" s="126"/>
+      <c r="J27" s="126"/>
+      <c r="K27" s="126"/>
+      <c r="L27" s="126"/>
+      <c r="M27" s="120"/>
+    </row>
+    <row r="28" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="134"/>
+      <c r="B28" s="135" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="13">
+      <c r="C28" s="135"/>
+      <c r="D28" s="135"/>
+      <c r="E28" s="136">
         <f>E26+E27</f>
         <v>274276.25</v>
       </c>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
+      <c r="F28" s="140"/>
+      <c r="G28" s="140"/>
+      <c r="H28" s="130"/>
+      <c r="I28" s="130"/>
+      <c r="J28" s="130"/>
+      <c r="K28" s="130"/>
+      <c r="L28" s="130"/>
+      <c r="M28" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7353,153 +7678,153 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A64E53E-4687-417C-9D55-21469B4B1E62}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="K24" sqref="J24:K24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="20.44140625" style="104" customWidth="1"/>
+    <col min="1" max="4" width="20.44140625" style="90" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="117" t="s">
+      <c r="B1" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="119" t="s">
+      <c r="D1" s="105" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="105">
+      <c r="B2" s="91">
         <v>270010</v>
       </c>
-      <c r="C2" s="106">
+      <c r="C2" s="92">
         <v>50165</v>
       </c>
-      <c r="D2" s="113">
+      <c r="D2" s="99">
         <f t="shared" ref="D2:D5" si="0">SUM(B2:C2)</f>
         <v>320175</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="112" t="s">
+      <c r="A3" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="107">
+      <c r="B3" s="93">
         <v>243880</v>
       </c>
-      <c r="C3" s="108">
+      <c r="C3" s="94">
         <v>47255</v>
       </c>
-      <c r="D3" s="114">
+      <c r="D3" s="100">
         <f t="shared" si="0"/>
         <v>291135</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="112" t="s">
+      <c r="A4" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="107">
+      <c r="B4" s="93">
         <v>286285</v>
       </c>
-      <c r="C4" s="108">
+      <c r="C4" s="94">
         <v>61040</v>
       </c>
-      <c r="D4" s="114">
+      <c r="D4" s="100">
         <f t="shared" si="0"/>
         <v>347325</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="112" t="s">
+      <c r="A5" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="124">
+      <c r="B5" s="110">
         <f>AVERAGE(B2:B4)</f>
         <v>266725</v>
       </c>
-      <c r="C5" s="125">
+      <c r="C5" s="111">
         <f>AVERAGE(C2:C4)</f>
         <v>52820</v>
       </c>
-      <c r="D5" s="126">
+      <c r="D5" s="112">
         <f t="shared" si="0"/>
         <v>319545</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="112" t="s">
+      <c r="A6" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="109">
+      <c r="B6" s="95">
         <v>261450</v>
       </c>
-      <c r="C6" s="110">
+      <c r="C6" s="96">
         <v>12826.25</v>
       </c>
-      <c r="D6" s="115">
+      <c r="D6" s="101">
         <f>SUM(B6:C6)</f>
         <v>274276.25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="112" t="s">
+      <c r="A7" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="121">
+      <c r="B7" s="107">
         <f>B5-B6</f>
         <v>5275</v>
       </c>
-      <c r="C7" s="122">
+      <c r="C7" s="108">
         <f>C5-(C6*2)</f>
         <v>27167.5</v>
       </c>
-      <c r="D7" s="123">
-        <f t="shared" ref="C7:D7" si="1">D5-D6</f>
+      <c r="D7" s="109">
+        <f t="shared" ref="D7" si="1">D5-D6</f>
         <v>45268.75</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="112" t="s">
+      <c r="A8" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="127">
+      <c r="B8" s="113">
         <f>((B6*100)/B5)/100</f>
         <v>0.98022307620208082</v>
       </c>
-      <c r="C8" s="128">
+      <c r="C8" s="114">
         <f t="shared" ref="C8:D8" si="2">((C6*100)/C5)/100</f>
         <v>0.24282942067398711</v>
       </c>
-      <c r="D8" s="129">
+      <c r="D8" s="115">
         <f t="shared" si="2"/>
         <v>0.85833372451454404</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="A9" s="120" t="s">
+      <c r="A9" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="130">
+      <c r="B9" s="116">
         <f>100-98</f>
         <v>2</v>
       </c>
-      <c r="C9" s="131">
+      <c r="C9" s="117">
         <f>100-24</f>
         <v>76</v>
       </c>
-      <c r="D9" s="132">
+      <c r="D9" s="118">
         <f>100-86</f>
         <v>14</v>
       </c>

</xml_diff>